<commit_message>
Update docs, add tests for SortedDeque
</commit_message>
<xml_diff>
--- a/specs.xlsx
+++ b/specs.xlsx
@@ -1,71 +1,83 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e3d7ce12028e4310/Documents/School/SYSC 3303/elevator/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zhiqiao\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="19" documentId="8_{2DCCEA50-0744-4F40-BC64-F162102FC853}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{5E18D73A-562F-4ED2-AF48-2FA5198AF9EC}"/>
   <bookViews>
-    <workbookView xWindow="11280" yWindow="684" windowWidth="17280" windowHeight="8820" xr2:uid="{39920257-C42B-4AEF-9AD7-B91C194AACE0}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8055"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
-  <si>
-    <t>starting floor</t>
-  </si>
-  <si>
-    <t>stopping floor</t>
-  </si>
-  <si>
-    <t>time spent (s)</t>
-  </si>
-  <si>
-    <t>floor #</t>
-  </si>
-  <si>
-    <t>height</t>
-  </si>
-  <si>
-    <t>steps</t>
-  </si>
-  <si>
-    <t>avg loading time</t>
-  </si>
-  <si>
-    <t>avg unloading time</t>
-  </si>
-  <si>
-    <t>avg speed</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="15">
+  <si>
+    <t>door close</t>
+  </si>
+  <si>
+    <t>door open</t>
+  </si>
+  <si>
+    <t>stay</t>
+  </si>
+  <si>
+    <t>stay(2 people drop)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Time  </t>
+  </si>
+  <si>
+    <t>Floor</t>
+  </si>
+  <si>
+    <t>Floor Button</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Car Button</t>
+  </si>
+  <si>
+    <t>up</t>
+  </si>
+  <si>
+    <t>car move</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>avg stay time</t>
+  </si>
+  <si>
+    <t>avg door open time</t>
+  </si>
+  <si>
+    <t>avg door close time</t>
+  </si>
+  <si>
+    <t>avg time move(1 floor)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="mm:ss.0;@"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -95,8 +107,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -131,7 +147,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -143,7 +159,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -190,23 +206,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -242,23 +241,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -410,56 +392,259 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CA501B9-4FBC-4D56-8114-7CF23FB017C0}">
-  <dimension ref="A1:G10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" customWidth="1"/>
+    <col min="2" max="2" width="6.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" customWidth="1"/>
+    <col min="6" max="6" width="22.7109375" customWidth="1"/>
+    <col min="7" max="7" width="12.85546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>4.6296296296296294E-5</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>1.5208333333333333E-4</v>
+      </c>
+      <c r="B3">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>5.99537037037037E-5</v>
+      </c>
+      <c r="B4">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="1">
+        <f xml:space="preserve"> (A9+A13+A17)/3</f>
+        <v>3.0054012345679011E-5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="B5"/>
+      <c r="F5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" s="1">
+        <f>(A5+A8+A12+A16)/4</f>
+        <v>6.7968749999999995E-5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>3.3680555555555555E-5</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="1">
+        <f>(A6+A10+A14+A18)/4</f>
+        <v>7.2019675925925924E-5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>3.9930555555555558E-5</v>
+      </c>
+      <c r="B7"/>
+      <c r="C7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" s="1">
+        <f>(A7+A11+A15)/3</f>
+        <v>3.6149691358024699E-5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>8.9583333333333333E-5</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>2.2337962962962963E-5</v>
+      </c>
+      <c r="B9"/>
+      <c r="C9" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>9.0625000000000007E-5</v>
+      </c>
+      <c r="B10"/>
+      <c r="C10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>3.4259259259259262E-5</v>
+      </c>
+      <c r="B11"/>
+      <c r="C11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>9.0740740740740734E-5</v>
+      </c>
+      <c r="B12">
+        <v>3</v>
+      </c>
+      <c r="C12" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>3.4259259259259262E-5</v>
+      </c>
+      <c r="B13"/>
+      <c r="C13" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>9.0740740740740734E-5</v>
+      </c>
+      <c r="B14"/>
+      <c r="C14" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>3.4259259259259262E-5</v>
+      </c>
+      <c r="B15"/>
+      <c r="C15" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>9.1550925925925928E-5</v>
+      </c>
+      <c r="B16">
+        <v>4</v>
+      </c>
+      <c r="C16" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>3.3564814814814815E-5</v>
+      </c>
+      <c r="B17"/>
+      <c r="C17" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>7.3032407407407399E-5</v>
+      </c>
+      <c r="B18"/>
+      <c r="C18" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>8</v>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>3.2754629629629628E-5</v>
+      </c>
+      <c r="B19"/>
+      <c r="C19" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <f>SUM(A6:A19)</f>
+        <v>7.9131944444444454E-4</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>